<commit_message>
Changed data values for use in testing / demo
</commit_message>
<xml_diff>
--- a/xlsx_test/test-spreadsheet3.xlsx
+++ b/xlsx_test/test-spreadsheet3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkrepp.AD\process-bp-count-spreadsheets\xlsx_text\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkrepp.AD\process-bp-count-spreadsheets\xlsx_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0F36BE-EAC5-4DBD-AEAB-230C5FB0F66D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905D4492-5E65-4D1B-AFED-E1972637E625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23256" yWindow="192" windowWidth="21600" windowHeight="11388" tabRatio="778" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
+    <workbookView xWindow="23664" yWindow="624" windowWidth="21600" windowHeight="11388" tabRatio="778" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="452">
   <si>
     <t>Municipality</t>
   </si>
@@ -1750,6 +1750,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1757,16 +1772,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1781,12 +1787,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2353,44 +2353,44 @@
       <c r="C2" s="7">
         <v>45238</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="22" t="s">
         <v>443</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="21" t="s">
+      <c r="E2" s="22"/>
+      <c r="F2" s="23" t="s">
         <v>331</v>
       </c>
-      <c r="G2" s="21"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="10"/>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="22" t="s">
         <v>304</v>
       </c>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="Q2" s="15" t="s">
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="Q2" s="20" t="s">
         <v>446</v>
       </c>
-      <c r="R2" s="16"/>
+      <c r="R2" s="21"/>
     </row>
     <row r="3" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>306</v>
       </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
       <c r="H3" s="10"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
       <c r="Q3" s="12" t="s">
         <v>447</v>
       </c>
@@ -2405,19 +2405,19 @@
       <c r="C4" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
       <c r="H4" s="10"/>
-      <c r="J4" s="22" t="s">
+      <c r="J4" s="24" t="s">
         <v>451</v>
       </c>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
       <c r="Q4" s="13" t="s">
         <v>448</v>
       </c>
@@ -2426,157 +2426,157 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="20" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
       <c r="H5" s="1">
         <f>VLOOKUP(D5,Columns!$D$3:$E$272,2,0)</f>
         <v>20030</v>
       </c>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
     </row>
     <row r="6" spans="2:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="18" t="s">
         <v>352</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="20" t="s">
+      <c r="C6" s="18"/>
+      <c r="D6" s="16" t="s">
         <v>428</v>
       </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="26" t="s">
+      <c r="E6" s="16"/>
+      <c r="F6" s="15" t="s">
         <v>450</v>
       </c>
-      <c r="G6" s="26"/>
+      <c r="G6" s="15"/>
       <c r="H6" s="1"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="17" t="s">
         <v>323</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="25"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="27"/>
       <c r="H7" s="1"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>324</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="20" t="s">
+      <c r="C8" s="17"/>
+      <c r="D8" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
       <c r="H8" s="2"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
     </row>
     <row r="9" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="18" t="s">
         <v>442</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
       <c r="H9" s="1"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>325</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="20" t="s">
+      <c r="C10" s="17"/>
+      <c r="D10" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
       <c r="H10" s="2"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="20" t="s">
+      <c r="C11" s="17"/>
+      <c r="D11" s="16" t="s">
         <v>427</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
       <c r="H11" s="1"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="20" t="s">
+      <c r="C12" s="17"/>
+      <c r="D12" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
       <c r="H12" s="1"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
     </row>
     <row r="14" spans="2:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
@@ -2585,17 +2585,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B11:C11"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B7:C7"/>
@@ -2612,6 +2601,17 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{B33F18CB-4361-4EA4-89CA-2CFFDEBFD17B}">
@@ -5343,7 +5343,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:H13"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5385,22 +5385,22 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5408,25 +5408,25 @@
         <v>0.26041666666666669</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5434,25 +5434,25 @@
         <v>0.27083333333333331</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -5460,25 +5460,25 @@
         <v>0.28125</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -5486,25 +5486,25 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
       <c r="G6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H6">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5515,22 +5515,22 @@
         <v>315</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G7">
         <v>6</v>
       </c>
       <c r="H7">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -5538,22 +5538,22 @@
         <v>0.3125</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H8">
         <v>7</v>
@@ -5564,22 +5564,22 @@
         <v>0.32291666666666669</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F9">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H9" t="s">
         <v>315</v>
@@ -5590,19 +5590,19 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E10">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F10">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G10" t="s">
         <v>315</v>
@@ -5616,16 +5616,16 @@
         <v>0.34375</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E11">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F11" t="s">
         <v>315</v>
@@ -5642,13 +5642,13 @@
         <v>0.35416666666666669</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D12">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E12" t="s">
         <v>315</v>
@@ -5668,10 +5668,10 @@
         <v>0.36458333333333331</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -5684,7 +5684,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H13"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5727,25 +5727,25 @@
         <v>0.375</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D2">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G2">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="H2">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5753,25 +5753,25 @@
         <v>0.38541666666666669</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G3">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="H3">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5779,25 +5779,25 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G4">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="H4">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -5805,25 +5805,25 @@
         <v>0.40625</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="H5">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -5831,25 +5831,25 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F6">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="H6">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5857,25 +5857,25 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G7">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="H7">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -5883,25 +5883,25 @@
         <v>0.4375</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D8">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F8">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G8">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="H8">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -5909,25 +5909,25 @@
         <v>0.44791666666666669</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D9">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F9">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G9">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="H9">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -5935,25 +5935,25 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D10">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F10">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G10">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="H10">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -5961,25 +5961,25 @@
         <v>0.46875</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D11">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F11">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G11">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="H11">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -5987,25 +5987,25 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D12">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F12">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G12">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="H12">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -6013,25 +6013,25 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="B13">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D13">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G13">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="H13">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -6044,7 +6044,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6086,25 +6086,25 @@
         <v>0.5</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E2">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F2">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H2">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -6112,25 +6112,25 @@
         <v>0.51041666666666663</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>315</v>
       </c>
       <c r="D3">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E3">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F3">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -6138,25 +6138,25 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="B4">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
         <v>315</v>
       </c>
       <c r="E4">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F4">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="H4">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -6164,25 +6164,25 @@
         <v>0.53125</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C5">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D5">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
         <v>315</v>
       </c>
       <c r="F5">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -6190,25 +6190,22 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="B6">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C6">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E6">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>315</v>
+        <v>9</v>
       </c>
       <c r="G6">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="H6">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -6216,25 +6213,25 @@
         <v>0.55208333333333337</v>
       </c>
       <c r="B7">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D7">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E7">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="G7" t="s">
         <v>315</v>
       </c>
       <c r="H7">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -6242,22 +6239,22 @@
         <v>0.5625</v>
       </c>
       <c r="B8">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D8">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E8">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F8">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="H8" t="s">
         <v>315</v>
@@ -6268,25 +6265,22 @@
         <v>0.57291666666666663</v>
       </c>
       <c r="B9">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C9">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D9">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E9">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F9">
-        <v>19</v>
-      </c>
-      <c r="G9" t="s">
-        <v>315</v>
+        <v>1</v>
       </c>
       <c r="H9">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -6294,25 +6288,25 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="B10">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C10">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D10">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E10">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F10" t="s">
         <v>315</v>
       </c>
       <c r="G10">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="H10">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -6320,25 +6314,25 @@
         <v>0.59375</v>
       </c>
       <c r="B11">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D11">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s">
         <v>315</v>
       </c>
       <c r="F11">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="H11">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -6346,25 +6340,25 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="B12">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C12">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
         <v>315</v>
       </c>
       <c r="E12">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="F12">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="H12">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -6372,25 +6366,25 @@
         <v>0.61458333333333337</v>
       </c>
       <c r="B13">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
         <v>315</v>
       </c>
       <c r="D13">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E13">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="F13">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="H13">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -6403,7 +6397,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6444,25 +6438,25 @@
         <v>0.625</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>315</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
         <v>315</v>
       </c>
       <c r="F2">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="G2" t="s">
         <v>315</v>
       </c>
       <c r="H2">
-        <v>100</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -6473,19 +6467,19 @@
         <v>315</v>
       </c>
       <c r="C3">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
         <v>315</v>
       </c>
       <c r="E3">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
         <v>315</v>
       </c>
       <c r="G3">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="H3" t="s">
         <v>315</v>
@@ -6496,25 +6490,25 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="B4">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>315</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
         <v>315</v>
       </c>
       <c r="F4">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="G4" t="s">
         <v>315</v>
       </c>
       <c r="H4">
-        <v>100</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -6525,19 +6519,19 @@
         <v>315</v>
       </c>
       <c r="C5">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
         <v>315</v>
       </c>
       <c r="E5">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="F5" t="s">
         <v>315</v>
       </c>
       <c r="G5">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="H5" t="s">
         <v>315</v>
@@ -6548,25 +6542,25 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="B6">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>315</v>
       </c>
       <c r="D6">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
         <v>315</v>
       </c>
       <c r="F6">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="G6" t="s">
         <v>315</v>
       </c>
       <c r="H6">
-        <v>100</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -6577,19 +6571,19 @@
         <v>315</v>
       </c>
       <c r="C7">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
         <v>315</v>
       </c>
       <c r="E7">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="F7" t="s">
         <v>315</v>
       </c>
       <c r="G7">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="H7" t="s">
         <v>315</v>
@@ -6600,25 +6594,25 @@
         <v>0.6875</v>
       </c>
       <c r="B8">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
         <v>315</v>
       </c>
       <c r="D8">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E8" t="s">
         <v>315</v>
       </c>
       <c r="F8">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="G8" t="s">
         <v>315</v>
       </c>
       <c r="H8">
-        <v>100</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -6629,19 +6623,19 @@
         <v>315</v>
       </c>
       <c r="C9">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
         <v>315</v>
       </c>
       <c r="E9">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="F9" t="s">
         <v>315</v>
       </c>
       <c r="G9">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="H9" t="s">
         <v>315</v>
@@ -6652,25 +6646,25 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="B10">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
         <v>315</v>
       </c>
       <c r="D10">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E10" t="s">
         <v>315</v>
       </c>
       <c r="F10">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="G10" t="s">
         <v>315</v>
       </c>
       <c r="H10">
-        <v>100</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -6681,19 +6675,19 @@
         <v>315</v>
       </c>
       <c r="C11">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
         <v>315</v>
       </c>
       <c r="E11">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="F11" t="s">
         <v>315</v>
       </c>
       <c r="G11">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="H11" t="s">
         <v>315</v>
@@ -6704,25 +6698,25 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="B12">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
         <v>315</v>
       </c>
       <c r="D12">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E12" t="s">
         <v>315</v>
       </c>
       <c r="F12">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="G12" t="s">
         <v>315</v>
       </c>
       <c r="H12">
-        <v>100</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -6733,19 +6727,19 @@
         <v>315</v>
       </c>
       <c r="C13">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
         <v>315</v>
       </c>
       <c r="E13">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="F13" t="s">
         <v>315</v>
       </c>
       <c r="G13">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="H13" t="s">
         <v>315</v>
@@ -6761,7 +6755,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6802,25 +6796,25 @@
         <v>0.75</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -6828,13 +6822,13 @@
         <v>0.76041666666666663</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E3">
         <v>5</v>
@@ -6854,25 +6848,25 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>5</v>
       </c>
       <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
         <v>6</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>7</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>8</v>
-      </c>
-      <c r="H4">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -6880,25 +6874,25 @@
         <v>0.78125</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>5</v>
       </c>
       <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
         <v>6</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>7</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>8</v>
-      </c>
-      <c r="G5">
-        <v>9</v>
-      </c>
-      <c r="H5">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -6909,22 +6903,22 @@
         <v>5</v>
       </c>
       <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
         <v>6</v>
       </c>
-      <c r="D6">
+      <c r="G6">
         <v>7</v>
       </c>
-      <c r="E6">
+      <c r="H6">
         <v>8</v>
-      </c>
-      <c r="F6">
-        <v>9</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="H6">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -6932,25 +6926,25 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="G7">
         <v>7</v>
       </c>
-      <c r="D7">
+      <c r="H7">
         <v>8</v>
-      </c>
-      <c r="E7">
-        <v>9</v>
-      </c>
-      <c r="F7">
-        <v>10</v>
-      </c>
-      <c r="G7">
-        <v>11</v>
-      </c>
-      <c r="H7">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -6958,25 +6952,25 @@
         <v>0.8125</v>
       </c>
       <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="H8">
         <v>8</v>
-      </c>
-      <c r="D8">
-        <v>9</v>
-      </c>
-      <c r="E8">
-        <v>10</v>
-      </c>
-      <c r="F8">
-        <v>11</v>
-      </c>
-      <c r="G8">
-        <v>12</v>
-      </c>
-      <c r="H8">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -6984,22 +6978,22 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
         <v>8</v>
-      </c>
-      <c r="D9">
-        <v>10</v>
-      </c>
-      <c r="E9">
-        <v>11</v>
-      </c>
-      <c r="F9">
-        <v>12</v>
-      </c>
-      <c r="G9">
-        <v>13</v>
-      </c>
-      <c r="H9">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -7007,22 +7001,22 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C10">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E10">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F10">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G10">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="H10">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -7030,25 +7024,25 @@
         <v>0.84375</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C11">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D11">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E11" t="s">
         <v>315</v>
       </c>
       <c r="F11">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G11">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H11">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -7056,22 +7050,22 @@
         <v>0.85416666666666663</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C12">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D12">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E12">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G12">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="H12">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -7079,22 +7073,22 @@
         <v>0.86458333333333337</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C13">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D13">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E13">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F13">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="H13">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -7150,7 +7144,7 @@
         <v>0.875</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -7158,7 +7152,7 @@
         <v>0.88541666666666663</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -7166,7 +7160,7 @@
         <v>0.89583333333333337</v>
       </c>
       <c r="D4">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -7174,7 +7168,7 @@
         <v>0.90625</v>
       </c>
       <c r="E5">
-        <v>40</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -7182,7 +7176,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="F6">
-        <v>50</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -7190,7 +7184,7 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="G7">
-        <v>60</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -7198,7 +7192,7 @@
         <v>0.9375</v>
       </c>
       <c r="H8">
-        <v>70</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -7206,7 +7200,7 @@
         <v>0.94791666666666663</v>
       </c>
       <c r="G9">
-        <v>80</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -7214,7 +7208,7 @@
         <v>0.95833333333333337</v>
       </c>
       <c r="F10">
-        <v>90</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -7222,7 +7216,7 @@
         <v>0.96875</v>
       </c>
       <c r="E11">
-        <v>100</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -7230,7 +7224,7 @@
         <v>0.97916666666666663</v>
       </c>
       <c r="D12">
-        <v>110</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -7238,7 +7232,7 @@
         <v>0.98958333333333337</v>
       </c>
       <c r="C13">
-        <v>120</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -7293,7 +7287,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -7301,7 +7295,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="C3">
-        <v>200</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -7309,7 +7303,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D4">
-        <v>300</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -7317,7 +7311,7 @@
         <v>3.125E-2</v>
       </c>
       <c r="E5">
-        <v>400</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>315</v>
@@ -7328,7 +7322,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F6">
-        <v>500</v>
+        <v>1</v>
       </c>
       <c r="G6" t="s">
         <v>315</v>
@@ -7339,10 +7333,10 @@
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="G7">
-        <v>600</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>700</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -7350,7 +7344,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="G8">
-        <v>600</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -7358,7 +7352,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
       <c r="F9">
-        <v>500</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -7366,7 +7360,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E10">
-        <v>400</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -7374,7 +7368,7 @@
         <v>9.375E-2</v>
       </c>
       <c r="D11">
-        <v>388</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -7382,7 +7376,7 @@
         <v>0.10416666666666667</v>
       </c>
       <c r="C12">
-        <v>200</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -7390,7 +7384,7 @@
         <v>0.11458333333333333</v>
       </c>
       <c r="B13">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -7444,25 +7438,25 @@
         <v>0.125</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -7470,25 +7464,25 @@
         <v>0.13541666666666666</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -7496,25 +7490,25 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -7522,25 +7516,25 @@
         <v>0.15625</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -7548,25 +7542,25 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -7574,25 +7568,25 @@
         <v>0.17708333333333334</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -7600,25 +7594,25 @@
         <v>0.1875</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -7626,25 +7620,25 @@
         <v>0.19791666666666666</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -7652,25 +7646,25 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -7678,25 +7672,25 @@
         <v>0.21875</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -7704,25 +7698,25 @@
         <v>0.22916666666666666</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -7730,25 +7724,25 @@
         <v>0.23958333333333334</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>